<commit_message>
Elimino ejercicio de modificar la metrica de puntos pues fallaba en PCs en idioma español.
</commit_message>
<xml_diff>
--- a/Materiales/Especificaciones.xlsx
+++ b/Materiales/Especificaciones.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\sm.vb.diseno-con-pruebas-unitarias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\sm.vb.diseno-con-pruebas-unitarias\Materiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" state="hidden" r:id="rId1"/>
@@ -111,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D73" authorId="0" shapeId="0">
+    <comment ref="D59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="260">
   <si>
     <t>Genere la métrica de puntos</t>
   </si>
@@ -509,12 +509,6 @@
     <t>Podría no haber información disponible</t>
   </si>
   <si>
-    <t>89% 9.5|8.5</t>
-  </si>
-  <si>
-    <t>No hay métrica 10|0</t>
-  </si>
-  <si>
     <t>La fórmula de la métrica de tiempo efectivo es DiasNoEfectivos / CapacidadDelEquipo</t>
   </si>
   <si>
@@ -938,9 +932,6 @@
     <t>95% 95|100</t>
   </si>
   <si>
-    <t>91% 99|90</t>
-  </si>
-  <si>
     <t>se valida una iteración con &lt;puntos planificados&gt;, &lt;puntos terminados&gt;, &lt;capacidad del equipo&gt; y &lt;tiempo no efectivo&gt;</t>
   </si>
   <si>
@@ -998,16 +989,10 @@
     <t>Ejercicio: utilice la clase Iteracion con las tres propiedades nuevas.</t>
   </si>
   <si>
-    <t>Modifique la métrica de puntos</t>
-  </si>
-  <si>
     <t>Si no hay informacion de puntos disponible no se validan</t>
   </si>
   <si>
     <t>Ejercicio: Utilice una clase "Iteracion" con tres propiedades.</t>
-  </si>
-  <si>
-    <t>Ejercicio: Utilice una clase "Iteracion"</t>
   </si>
   <si>
     <t>Utilice la regla de negocio que obtiene la métrica para una sola iteración.</t>
@@ -1574,16 +1559,7 @@
     <cellStyle name="Note" xfId="7" builtinId="10"/>
     <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
+  <dxfs count="77">
     <dxf>
       <font>
         <b val="0"/>
@@ -2829,26 +2805,13 @@
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <b/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -3040,8 +3003,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="78"/>
-      <tableStyleElement type="headerRow" dxfId="77"/>
+      <tableStyleElement type="wholeTable" dxfId="76"/>
+      <tableStyleElement type="headerRow" dxfId="75"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3069,91 +3032,77 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B15:F19" totalsRowShown="0">
-  <autoFilter ref="B15:F19"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="50"/>
-    <tableColumn id="2" name="Numero"/>
-    <tableColumn id="3" name="Fecha inicial"/>
-    <tableColumn id="4" name="Fecha final"/>
-    <tableColumn id="5" name="Es válida o no"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B6:C8" totalsRowShown="0">
+  <autoFilter ref="B6:C8"/>
+  <tableColumns count="2">
+    <tableColumn id="2" name="Fecha de inicio" dataDxfId="47"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table168" displayName="Table168" ref="B28:I47" totalsRowShown="0">
+  <autoFilter ref="B28:I47"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Ejemplo" dataDxfId="45"/>
+    <tableColumn id="7" name="Hay informacion de puntos disponible" dataDxfId="44"/>
+    <tableColumn id="2" name="Puntos planificados" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Puntos terminados" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Hay informacion de dias disponible"/>
+    <tableColumn id="4" name="Capacidad del equipo" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Días no efectivos"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B6:C8" totalsRowShown="0">
-  <autoFilter ref="B6:C8"/>
-  <tableColumns count="2">
-    <tableColumn id="2" name="Fecha de inicio" dataDxfId="49"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table168" displayName="Table168" ref="B28:I47" totalsRowShown="0">
-  <autoFilter ref="B28:I47"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="47"/>
-    <tableColumn id="7" name="Hay informacion de puntos disponible" dataDxfId="46"/>
-    <tableColumn id="2" name="Puntos planificados" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Puntos terminados" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Hay informacion de dias disponible"/>
-    <tableColumn id="4" name="Capacidad del equipo" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Días no efectivos"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1689" displayName="Table1689" ref="B57:G63" totalsRowShown="0">
+  <autoFilter ref="B57:G63"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Ejemplo" dataDxfId="42"/>
+    <tableColumn id="7" name="Fecha actual" dataDxfId="41"/>
+    <tableColumn id="2" name="Fecha de reporte" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Total de incidentes" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Descripción" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1689" displayName="Table1689" ref="B57:G63" totalsRowShown="0">
-  <autoFilter ref="B57:G63"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="44"/>
-    <tableColumn id="7" name="Fecha actual" dataDxfId="43"/>
-    <tableColumn id="2" name="Fecha de reporte" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Total de incidentes" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Descripción" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="B8:D11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Puntos planificados" dataDxfId="36"/>
+    <tableColumn id="2" name="Puntos terminados" dataDxfId="35"/>
+    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="34"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
-  <autoFilter ref="B8:D11"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Puntos planificados" dataDxfId="38"/>
-    <tableColumn id="2" name="Puntos terminados" dataDxfId="37"/>
-    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5" displayName="Table5" ref="B14:B17" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+  <autoFilter ref="B14:B17"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Métricas de puntos" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5" displayName="Table5" ref="B14:B17" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="B14:B17"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Métricas de puntos" dataDxfId="32"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table412" displayName="Table412" ref="B24:F25" totalsRowShown="0">
   <autoFilter ref="B24:F25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="31"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="30"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="29"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="28"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
@@ -3161,7 +3110,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A9:B12" totalsRowShown="0">
   <autoFilter ref="A9:B12"/>
   <tableColumns count="2">
@@ -3172,7 +3121,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="B40:E41" totalsRowShown="0">
   <autoFilter ref="B40:E41"/>
   <tableColumns count="4">
@@ -3185,12 +3134,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="B32:F33" totalsRowShown="0">
   <autoFilter ref="B32:F33"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="ISIN" dataDxfId="29"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="28"/>
+    <tableColumn id="5" name="ISIN" dataDxfId="27"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="26"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -3199,18 +3148,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
-  <autoFilter ref="C57:D64"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="76"/>
-    <tableColumn id="2" name="Puntos de la historia" dataDxfId="75"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table26" displayName="Table26" ref="B36:C37" totalsRowShown="0">
   <autoFilter ref="B36:C37"/>
   <tableColumns count="2">
@@ -3221,25 +3159,36 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B20:J21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="B20:J21"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Numero" dataDxfId="24"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="23"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="22"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="21"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="20"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="19"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="18"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="17"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="16"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
+  <autoFilter ref="C57:D64"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="74"/>
+    <tableColumn id="2" name="Puntos de la historia" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B20:J21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="B20:J21"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Numero" dataDxfId="22"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="21"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="20"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="19"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="18"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="17"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="16"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="15"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table2431" displayName="Table2431" ref="B34:E37" totalsRowShown="0">
   <autoFilter ref="B34:E37"/>
   <tableColumns count="4">
@@ -3252,12 +3201,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table2532" displayName="Table2532" ref="B22:F25" totalsRowShown="0">
   <autoFilter ref="B22:F25"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="ISIN" dataDxfId="15"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="14"/>
+    <tableColumn id="5" name="ISIN" dataDxfId="13"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="12"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -3266,7 +3215,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table2633" displayName="Table2633" ref="B28:C31" totalsRowShown="0">
   <autoFilter ref="B28:C31"/>
   <tableColumns count="2">
@@ -3277,31 +3226,31 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B6:J9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B6:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="B6:J9"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Numero"/>
-    <tableColumn id="2" name="fecha inicial" dataDxfId="11"/>
-    <tableColumn id="3" name="fecha final" dataDxfId="10"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="9"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="8"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="7"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="6"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="5"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="4"/>
+    <tableColumn id="2" name="fecha inicial" dataDxfId="9"/>
+    <tableColumn id="3" name="fecha final" dataDxfId="8"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="7"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="6"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="5"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="4"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="3"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table41224" displayName="Table41224" ref="B13:F16" totalsRowShown="0">
   <autoFilter ref="B13:F16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="3"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="2"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="1"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="0"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
@@ -3310,12 +3259,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="74" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="B69:D72"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="72"/>
-    <tableColumn id="2" name="Iteración" dataDxfId="71"/>
-    <tableColumn id="3" name="Velocidad" dataDxfId="70"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="70"/>
+    <tableColumn id="2" name="Iteración" dataDxfId="69"/>
+    <tableColumn id="3" name="Velocidad" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3325,7 +3274,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B43:F48" totalsRowShown="0">
   <autoFilter ref="B43:F48"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="69"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="67"/>
     <tableColumn id="2" name="Puntos planificados"/>
     <tableColumn id="3" name="Puntos terminados"/>
     <tableColumn id="4" name="Hay informacion de puntos disponible"/>
@@ -3336,22 +3285,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B58:F63" totalsRowShown="0">
-  <autoFilter ref="B58:F63"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="68"/>
-    <tableColumn id="6" name="Hay informacion de puntos disponible" dataDxfId="67"/>
-    <tableColumn id="2" name="Puntos planificados"/>
-    <tableColumn id="3" name="Puntos terminados"/>
-    <tableColumn id="5" name="Métrica de puntos"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B73:F77" totalsRowShown="0">
-  <autoFilter ref="B73:F77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B59:F63" totalsRowShown="0">
+  <autoFilter ref="B59:F63"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ejemplo" dataDxfId="66"/>
     <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="65"/>
@@ -3363,14 +3298,14 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="B23:G26" totalsRowShown="0">
   <autoFilter ref="B23:G26"/>
   <tableColumns count="6">
-    <tableColumn id="5" name="Ejemplo" dataDxfId="0"/>
-    <tableColumn id="6" name="Porcentaje de cobertura" dataDxfId="1"/>
-    <tableColumn id="4" name="Fecha actual" dataDxfId="64"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="63"/>
+    <tableColumn id="5" name="Ejemplo" dataDxfId="64"/>
+    <tableColumn id="6" name="Porcentaje de cobertura" dataDxfId="63"/>
+    <tableColumn id="4" name="Fecha actual" dataDxfId="62"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="61"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura revisado"/>
   </tableColumns>
@@ -3378,13 +3313,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="B11:D12" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="B11:D12" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="B11:D12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Precio limpio del vector de precios" dataDxfId="59" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Monto nominal del saldo" dataDxfId="58" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Valor de mercado" dataDxfId="57" dataCellStyle="Comma">
+    <tableColumn id="1" name="Precio limpio del vector de precios" dataDxfId="57" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Monto nominal del saldo" dataDxfId="56" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Valor de mercado" dataDxfId="55" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Precio limpio del vector de precios]*(Table28[Monto nominal del saldo]/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3392,19 +3327,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="B32:D33" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="B32:D33" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="B32:D33"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Valor de mercado" dataDxfId="53" dataCellStyle="Comma">
+    <tableColumn id="1" name="Valor de mercado" dataDxfId="51" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Precio limpio del vector de precios]*(Table28[Monto nominal del saldo]/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="52"/>
-    <tableColumn id="3" name="Aporte de garantía" dataDxfId="51" dataCellStyle="Comma">
+    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="50"/>
+    <tableColumn id="3" name="Aporte de garantía" dataDxfId="49" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table2830[Valor de mercado]*Table2830[Porcentaje de cobertura revisado]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B15:F19" totalsRowShown="0">
+  <autoFilter ref="B15:F19"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Ejemplo" dataDxfId="48"/>
+    <tableColumn id="2" name="Numero"/>
+    <tableColumn id="3" name="Fecha inicial"/>
+    <tableColumn id="4" name="Fecha final"/>
+    <tableColumn id="5" name="Es válida o no"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3688,33 +3637,33 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3724,10 +3673,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -3739,7 +3688,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
@@ -3752,10 +3701,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -3780,10 +3729,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -3808,7 +3757,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
@@ -3824,7 +3773,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3832,7 +3781,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3840,37 +3789,37 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3878,7 +3827,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,7 +3835,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3894,7 +3843,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3907,18 +3856,18 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C39">
         <v>1000</v>
@@ -3932,7 +3881,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40">
         <v>1000</v>
@@ -3946,7 +3895,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41">
         <v>1000</v>
@@ -3960,7 +3909,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42">
         <v>1000</v>
@@ -3974,65 +3923,65 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4103,10 +4052,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4114,7 +4063,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,15 +4071,15 @@
         <v>6</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C70">
         <v>4</v>
@@ -4141,7 +4090,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4152,7 +4101,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -4163,178 +4112,178 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" s="29" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="45" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="29" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4367,7 +4316,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -4377,87 +4326,87 @@
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4468,15 +4417,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -4487,24 +4434,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4518,10 +4465,10 @@
     </row>
     <row r="6" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -4530,7 +4477,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C7" s="8"/>
     </row>
@@ -4539,7 +4486,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C8" s="8"/>
     </row>
@@ -4556,13 +4503,13 @@
     <row r="11" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -4584,15 +4531,15 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4600,15 +4547,15 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4616,7 +4563,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4624,7 +4571,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4637,24 +4584,24 @@
         <v>6</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="47">
         <v>0.8</v>
@@ -4674,7 +4621,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="47">
         <v>0.8</v>
@@ -4694,7 +4641,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="46" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C26" s="47">
         <v>0.8</v>
@@ -4724,16 +4671,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -4745,13 +4692,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4774,7 +4721,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>0</v>
@@ -4788,7 +4735,7 @@
     </row>
     <row r="37" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4796,7 +4743,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4914,132 +4861,111 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B50" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="C50" s="48"/>
-    </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>17</v>
+      <c r="A51" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" t="s">
-        <v>52</v>
+      <c r="A53" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>6</v>
       </c>
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59">
-        <v>100</v>
-      </c>
-      <c r="E59">
-        <v>95</v>
-      </c>
-      <c r="F59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
         <v>12</v>
       </c>
       <c r="D60">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E60">
-        <v>90</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>164</v>
+        <v>5</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
         <v>12</v>
       </c>
       <c r="D61">
-        <v>9.5</v>
+        <v>99</v>
       </c>
       <c r="E61">
-        <v>8.5</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>21</v>
+        <v>5.67</v>
+      </c>
+      <c r="F61" s="1">
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
       </c>
       <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62">
         <v>0</v>
       </c>
-      <c r="E62">
-        <v>10</v>
-      </c>
-      <c r="F62" t="s">
-        <v>22</v>
+      <c r="F62" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5059,151 +4985,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" t="s">
-        <v>28</v>
-      </c>
-      <c r="D73" t="s">
-        <v>26</v>
-      </c>
-      <c r="E73" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74">
-        <v>100</v>
-      </c>
-      <c r="E74">
-        <v>5</v>
-      </c>
-      <c r="F74" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" t="s">
-        <v>12</v>
-      </c>
-      <c r="D75">
-        <v>99</v>
-      </c>
-      <c r="E75">
-        <v>5.67</v>
-      </c>
-      <c r="F75" s="1">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76">
-        <v>100</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C77" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E79" s="29"/>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B50:C50"/>
+  <mergeCells count="1">
     <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="6">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5231,33 +5031,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5086,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5294,7 +5094,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -5307,21 +5107,21 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -5333,12 +5133,12 @@
         <v>43042</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -5350,12 +5150,12 @@
         <v>43042</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -5367,12 +5167,12 @@
         <v>43037</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -5384,15 +5184,15 @@
         <v>43037</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C21" s="28"/>
     </row>
@@ -5404,7 +5204,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -5412,7 +5212,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -5434,21 +5234,21 @@
         <v>8</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H28" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>12</v>
@@ -5469,12 +5269,12 @@
         <v>20</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>13</v>
@@ -5495,12 +5295,12 @@
         <v>20</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -5521,12 +5321,12 @@
         <v>20</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -5547,10 +5347,10 @@
         <v>20</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -5561,7 +5361,7 @@
     </row>
     <row r="33" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -5582,12 +5382,12 @@
         <v>20</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -5608,12 +5408,12 @@
         <v>20</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="28" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -5634,12 +5434,12 @@
         <v>20</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -5660,12 +5460,12 @@
         <v>20</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -5686,12 +5486,12 @@
         <v>20</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -5712,12 +5512,12 @@
         <v>20</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="2:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -5738,12 +5538,12 @@
         <v>-1</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -5764,12 +5564,12 @@
         <v>20</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -5790,12 +5590,12 @@
         <v>0</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -5816,12 +5616,12 @@
         <v>20</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -5842,12 +5642,12 @@
         <v>20</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -5868,12 +5668,12 @@
         <v>-0.01</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -5894,12 +5694,12 @@
         <v>0</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -5920,12 +5720,12 @@
         <v>100.01</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -5946,15 +5746,15 @@
         <v>100</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B49" s="48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="48"/>
     </row>
@@ -5963,7 +5763,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -5971,7 +5771,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5979,7 +5779,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5992,24 +5792,24 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C58" s="12">
         <v>43042</v>
@@ -6021,15 +5821,15 @@
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C59" s="12">
         <v>43042</v>
@@ -6041,15 +5841,15 @@
         <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C60" s="12">
         <v>43042</v>
@@ -6061,15 +5861,15 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C61" s="12">
         <v>43042</v>
@@ -6082,12 +5882,12 @@
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
@@ -6097,7 +5897,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="12">
         <v>43042</v>
@@ -6109,10 +5909,10 @@
         <v>8</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -6149,33 +5949,33 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6186,7 +5986,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6211,7 +6011,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -6244,13 +6044,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6303,25 +6103,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6329,7 +6129,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6337,28 +6137,28 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8">
         <v>43399</v>
@@ -6366,7 +6166,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" s="8">
         <v>43393</v>
@@ -6374,7 +6174,7 @@
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -6386,10 +6186,10 @@
     </row>
     <row r="16" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -6423,18 +6223,18 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>9</v>
@@ -6446,13 +6246,13 @@
         <v>8</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -6500,24 +6300,24 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -6531,7 +6331,7 @@
         <v>43028</v>
       </c>
       <c r="E25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F25" s="1">
         <v>0.05</v>
@@ -6539,10 +6339,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -6550,37 +6350,37 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" t="s">
         <v>141</v>
-      </c>
-      <c r="D32" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C33" s="8">
         <v>42527</v>
@@ -6597,23 +6397,23 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" t="s">
         <v>144</v>
-      </c>
-      <c r="C36" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C37" s="7">
         <v>3578000</v>
@@ -6624,26 +6424,26 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C41">
         <v>0.8</v>
@@ -6657,7 +6457,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -6700,17 +6500,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="48"/>
@@ -6718,21 +6518,21 @@
     </row>
     <row r="5" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>9</v>
@@ -6744,13 +6544,13 @@
         <v>8</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6846,7 +6646,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6854,24 +6654,24 @@
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6885,7 +6685,7 @@
         <v>43028</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F14" s="1">
         <v>0.05</v>
@@ -6928,10 +6728,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -6939,37 +6739,37 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
         <v>141</v>
-      </c>
-      <c r="D22" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C23" s="8">
         <v>42527</v>
@@ -6986,7 +6786,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C24" s="8">
         <v>42370</v>
@@ -7003,7 +6803,7 @@
     </row>
     <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C25" s="8">
         <v>42005</v>
@@ -7020,23 +6820,23 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" t="s">
         <v>144</v>
-      </c>
-      <c r="C28" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C29" s="7">
         <v>3578000</v>
@@ -7044,7 +6844,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C30" s="7">
         <v>4578000</v>
@@ -7052,7 +6852,7 @@
     </row>
     <row r="31" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C31" s="7">
         <v>6576000</v>
@@ -7063,26 +6863,26 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C35">
         <v>0.8</v>
@@ -7096,7 +6896,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -7112,7 +6912,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C37" s="29">
         <v>0</v>

</xml_diff>

<commit_message>
Corrijo compilacion de algoritmo de la estructura de datos de las metricas de la iteracion.
</commit_message>
<xml_diff>
--- a/Materiales/Especificaciones.xlsx
+++ b/Materiales/Especificaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" state="hidden" r:id="rId1"/>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="258">
   <si>
     <t>Genere la métrica de puntos</t>
   </si>
@@ -929,9 +929,6 @@
     <t>HDA000000000002</t>
   </si>
   <si>
-    <t>95% 95|100</t>
-  </si>
-  <si>
     <t>se valida una iteración con &lt;puntos planificados&gt;, &lt;puntos terminados&gt;, &lt;capacidad del equipo&gt; y &lt;tiempo no efectivo&gt;</t>
   </si>
   <si>
@@ -1110,9 +1107,6 @@
   </si>
   <si>
     <t>Genere la valoración de una emisión en colones</t>
-  </si>
-  <si>
-    <t>80% 8|10</t>
   </si>
   <si>
     <t>se genera las metricas de la iteración</t>
@@ -3843,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,7 +3856,7 @@
         <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3931,7 +3925,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -4151,139 +4145,139 @@
     <row r="83" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" s="29" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="45" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="29" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -4316,7 +4310,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -4326,87 +4320,87 @@
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4419,7 +4413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4468,7 +4462,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -4477,7 +4471,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C7" s="8"/>
     </row>
@@ -4486,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C8" s="8"/>
     </row>
@@ -4539,7 +4533,7 @@
     </row>
     <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4735,7 +4729,7 @@
     </row>
     <row r="37" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4876,7 +4870,7 @@
     </row>
     <row r="53" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -4914,7 +4908,7 @@
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5048,7 +5042,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5192,7 +5186,7 @@
         <v>134</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C21" s="28"/>
     </row>
@@ -5204,7 +5198,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -5240,7 +5234,7 @@
         <v>24</v>
       </c>
       <c r="H28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I28" t="s">
         <v>41</v>
@@ -5274,7 +5268,7 @@
     </row>
     <row r="30" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>13</v>
@@ -5300,7 +5294,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -5326,7 +5320,7 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -5350,7 +5344,7 @@
         <v>39</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -5361,7 +5355,7 @@
     </row>
     <row r="33" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -5387,7 +5381,7 @@
     </row>
     <row r="34" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -5413,7 +5407,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -5439,7 +5433,7 @@
     </row>
     <row r="36" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -5465,7 +5459,7 @@
     </row>
     <row r="37" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -5491,7 +5485,7 @@
     </row>
     <row r="38" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -5517,7 +5511,7 @@
     </row>
     <row r="39" spans="2:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -5543,7 +5537,7 @@
     </row>
     <row r="40" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -5569,7 +5563,7 @@
     </row>
     <row r="41" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -5595,7 +5589,7 @@
     </row>
     <row r="42" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -5621,7 +5615,7 @@
     </row>
     <row r="43" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -5647,7 +5641,7 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -5673,7 +5667,7 @@
     </row>
     <row r="45" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -5699,7 +5693,7 @@
     </row>
     <row r="46" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -5725,7 +5719,7 @@
     </row>
     <row r="47" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -5887,7 +5881,7 @@
     </row>
     <row r="62" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
@@ -5959,7 +5953,7 @@
         <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5967,7 +5961,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5986,7 +5980,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6011,7 +6005,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -6044,13 +6038,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6084,8 +6078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,7 +6097,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -6174,7 +6168,7 @@
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -6189,7 +6183,7 @@
         <v>134</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -6223,7 +6217,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -6300,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6330,8 +6324,8 @@
       <c r="D25" s="35">
         <v>43028</v>
       </c>
-      <c r="E25" t="s">
-        <v>161</v>
+      <c r="E25" s="1">
+        <v>0.95</v>
       </c>
       <c r="F25" s="1">
         <v>0.05</v>
@@ -6342,7 +6336,7 @@
         <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -6457,7 +6451,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -6480,9 +6474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6500,7 +6492,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -6510,7 +6502,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="48"/>
@@ -6521,7 +6513,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6529,10 +6521,10 @@
         <v>36</v>
       </c>
       <c r="C6" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>208</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>209</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>9</v>
@@ -6646,7 +6638,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6654,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6684,8 +6676,8 @@
       <c r="D14" s="35">
         <v>43028</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>222</v>
+      <c r="E14" s="1">
+        <v>0.8</v>
       </c>
       <c r="F14" s="1">
         <v>0.05</v>
@@ -6731,7 +6723,7 @@
         <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -6803,7 +6795,7 @@
     </row>
     <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C25" s="8">
         <v>42005</v>
@@ -6852,7 +6844,7 @@
     </row>
     <row r="31" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C31" s="7">
         <v>6576000</v>
@@ -6912,7 +6904,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C37" s="29">
         <v>0</v>

</xml_diff>